<commit_message>
Re-draw model to within and between
</commit_message>
<xml_diff>
--- a/Model building/Missing table.xlsx
+++ b/Model building/Missing table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\pc\Dokumenter\MSc\Thesis\Model building\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{532CE266-60FF-4580-9D7F-A01B81F6F78C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3590F996-51EB-4689-A531-6A914F141058}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11456,7 +11456,7 @@
   <dimension ref="A1:V43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="Q31" sqref="Q31"/>
+      <selection activeCell="M36" sqref="M36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>